<commit_message>
corrected reference designators, indented engineering data
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CE07SHSP_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_CE07SHSP_00001.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\# OOI_Asset_Management\CE_mod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="588" yWindow="240" windowWidth="25608" windowHeight="16068" tabRatio="579"/>
+    <workbookView xWindow="585" yWindow="240" windowWidth="25605" windowHeight="16065" tabRatio="579" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -2291,28 +2291,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" customWidth="1"/>
-    <col min="13" max="13" width="15.109375" customWidth="1"/>
-    <col min="14" max="14" width="13.88671875" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="6" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>99</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -2393,93 +2393,93 @@
         <v>-124.56432</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="12"/>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D4" s="10"/>
       <c r="E4" s="11"/>
       <c r="F4" s="12"/>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D5" s="10"/>
       <c r="E5" s="11"/>
       <c r="F5" s="12"/>
       <c r="G5" s="11"/>
       <c r="M5" s="49"/>
     </row>
-    <row r="6" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D6" s="10"/>
       <c r="E6" s="11"/>
       <c r="F6" s="12"/>
       <c r="G6" s="11"/>
       <c r="M6" s="49"/>
     </row>
-    <row r="7" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D7" s="10"/>
       <c r="E7" s="11"/>
       <c r="F7" s="12"/>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D8" s="10"/>
       <c r="E8" s="11"/>
       <c r="F8" s="12"/>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D9" s="10"/>
       <c r="E9" s="11"/>
       <c r="F9" s="12"/>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D10" s="10"/>
       <c r="E10" s="11"/>
       <c r="F10" s="12"/>
       <c r="G10" s="11"/>
     </row>
-    <row r="11" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D11" s="10"/>
       <c r="E11" s="11"/>
       <c r="F11" s="12"/>
       <c r="G11" s="11"/>
     </row>
-    <row r="12" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D12" s="10"/>
       <c r="E12" s="11"/>
       <c r="F12" s="12"/>
       <c r="G12" s="11"/>
     </row>
-    <row r="13" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D13" s="10"/>
       <c r="E13" s="11"/>
       <c r="F13" s="12"/>
       <c r="G13" s="11"/>
     </row>
-    <row r="14" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D14" s="10"/>
       <c r="E14" s="11"/>
       <c r="F14" s="12"/>
       <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D15" s="10"/>
       <c r="E15" s="11"/>
       <c r="F15" s="12"/>
       <c r="G15" s="11"/>
     </row>
-    <row r="16" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D16" s="10"/>
       <c r="E16" s="11"/>
       <c r="F16" s="12"/>
       <c r="G16" s="11"/>
     </row>
-    <row r="17" spans="4:7" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:7" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D17" s="10"/>
       <c r="E17" s="11"/>
       <c r="F17" s="12"/>
@@ -2501,25 +2501,25 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" customWidth="1"/>
-    <col min="4" max="5" width="12.44140625" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="5" width="12.42578125" customWidth="1"/>
     <col min="6" max="6" width="17" style="7" customWidth="1"/>
-    <col min="7" max="7" width="37.88671875" customWidth="1"/>
-    <col min="8" max="8" width="57.33203125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="21.33203125" customWidth="1"/>
+    <col min="7" max="7" width="37.85546875" customWidth="1"/>
+    <col min="8" max="8" width="57.28515625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
@@ -2559,7 +2559,7 @@
       <c r="H2" s="20"/>
       <c r="I2" s="21"/>
     </row>
-    <row r="3" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>91</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>91</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>91</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
       <c r="B7" s="22"/>
       <c r="C7" s="27"/>
@@ -2686,7 +2686,7 @@
       <c r="H7" s="25"/>
       <c r="I7" s="20"/>
     </row>
-    <row r="8" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>89</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>89</v>
       </c>
@@ -2742,7 +2742,7 @@
       </c>
       <c r="I9" s="31"/>
     </row>
-    <row r="10" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>89</v>
       </c>
@@ -2769,7 +2769,7 @@
       </c>
       <c r="I10" s="31"/>
     </row>
-    <row r="11" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>89</v>
       </c>
@@ -2796,7 +2796,7 @@
       </c>
       <c r="I11" s="31"/>
     </row>
-    <row r="12" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>89</v>
       </c>
@@ -2823,7 +2823,7 @@
       </c>
       <c r="I12" s="31"/>
     </row>
-    <row r="13" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>89</v>
       </c>
@@ -2850,7 +2850,7 @@
       </c>
       <c r="I13" s="31"/>
     </row>
-    <row r="14" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>89</v>
       </c>
@@ -2877,7 +2877,7 @@
       </c>
       <c r="I14" s="31"/>
     </row>
-    <row r="15" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>89</v>
       </c>
@@ -2904,7 +2904,7 @@
       </c>
       <c r="I15" s="31"/>
     </row>
-    <row r="16" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
       <c r="B16" s="22"/>
       <c r="C16" s="27"/>
@@ -2915,7 +2915,7 @@
       <c r="H16" s="25"/>
       <c r="I16" s="20"/>
     </row>
-    <row r="17" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>92</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
         <v>92</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19"/>
       <c r="C19" s="27"/>
@@ -2984,7 +2984,7 @@
       <c r="H19" s="25"/>
       <c r="I19" s="20"/>
     </row>
-    <row r="20" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>93</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
         <v>93</v>
       </c>
@@ -3042,7 +3042,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
         <v>93</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>93</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
         <v>93</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
         <v>93</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
         <v>93</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
       <c r="B27" s="22"/>
       <c r="C27" s="27"/>
@@ -3198,7 +3198,7 @@
       <c r="H27" s="25"/>
       <c r="I27" s="20"/>
     </row>
-    <row r="28" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>94</v>
       </c>
@@ -3225,7 +3225,7 @@
       </c>
       <c r="I28" s="20"/>
     </row>
-    <row r="29" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
         <v>94</v>
       </c>
@@ -3252,7 +3252,7 @@
       </c>
       <c r="I29" s="20"/>
     </row>
-    <row r="30" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
         <v>94</v>
       </c>
@@ -3279,7 +3279,7 @@
       </c>
       <c r="I30" s="20"/>
     </row>
-    <row r="31" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
       <c r="B31"/>
       <c r="C31" s="27"/>
@@ -3290,7 +3290,7 @@
       <c r="H31" s="25"/>
       <c r="I31" s="20"/>
     </row>
-    <row r="32" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>95</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
         <v>95</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="26" t="s">
         <v>95</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="26" t="s">
         <v>95</v>
       </c>
@@ -3406,7 +3406,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
         <v>95</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
         <v>95</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
         <v>95</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
         <v>95</v>
       </c>
@@ -3522,7 +3522,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
         <v>95</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="26" t="s">
         <v>95</v>
       </c>
@@ -3580,7 +3580,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="26"/>
       <c r="B42" s="26"/>
       <c r="C42" s="27"/>
@@ -3591,7 +3591,7 @@
       <c r="H42" s="25"/>
       <c r="I42" s="20"/>
     </row>
-    <row r="43" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>96</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="26" t="s">
         <v>96</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
       <c r="B45" s="22"/>
       <c r="C45" s="27"/>
@@ -3660,7 +3660,7 @@
       <c r="H45" s="25"/>
       <c r="I45" s="20"/>
     </row>
-    <row r="46" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>97</v>
       </c>
@@ -3687,7 +3687,7 @@
       </c>
       <c r="I46" s="20"/>
     </row>
-    <row r="47" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="26" t="s">
         <v>97</v>
       </c>
@@ -3714,7 +3714,7 @@
       </c>
       <c r="I47" s="20"/>
     </row>
-    <row r="48" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="26" t="s">
         <v>97</v>
       </c>
@@ -3741,7 +3741,7 @@
       </c>
       <c r="I48" s="20"/>
     </row>
-    <row r="49" spans="1:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="33"/>
       <c r="B49" s="33"/>
       <c r="C49" s="33"/>
@@ -3751,34 +3751,34 @@
       <c r="G49" s="33"/>
       <c r="H49" s="34"/>
       <c r="I49" s="33"/>
-    </row>
-    <row r="50" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="35" t="s">
+      <c r="K49" s="7"/>
+    </row>
+    <row r="50" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I50" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="B50" t="s">
+      <c r="J50" t="s">
         <v>98</v>
       </c>
-      <c r="C50" s="23" t="s">
+      <c r="K50" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="D50" s="24">
+      <c r="L50" s="24">
         <v>1</v>
       </c>
-      <c r="E50" t="s">
+      <c r="M50" t="s">
         <v>101</v>
       </c>
-      <c r="F50" s="39" t="s">
+      <c r="N50" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="G50" s="20"/>
-      <c r="H50" s="36"/>
-      <c r="I50" s="20"/>
-    </row>
-    <row r="51" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="53" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+      <c r="O50" s="20"/>
+      <c r="P50" s="36"/>
+    </row>
+    <row r="51" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="34" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3799,9 +3799,9 @@
       <selection sqref="A1:AJ85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>4.6008E-2</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>-1.137E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4.2536999999999998E-2</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>-1.358E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4.3115000000000001E-2</v>
       </c>
@@ -4131,7 +4131,7 @@
         <v>-1.5838999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4.3878E-2</v>
       </c>
@@ -4241,7 +4241,7 @@
         <v>-1.8959E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4.3221000000000002E-2</v>
       </c>
@@ -4351,7 +4351,7 @@
         <v>-2.0358000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4.1510999999999999E-2</v>
       </c>
@@ -4461,7 +4461,7 @@
         <v>-1.9682000000000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3.7416999999999999E-2</v>
       </c>
@@ -4571,7 +4571,7 @@
         <v>-1.8426000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3.4866000000000001E-2</v>
       </c>
@@ -4681,7 +4681,7 @@
         <v>-1.6534E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3.1199999999999999E-2</v>
       </c>
@@ -4791,7 +4791,7 @@
         <v>-1.4978999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2.7692999999999999E-2</v>
       </c>
@@ -4901,7 +4901,7 @@
         <v>-1.3599999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2.4787E-2</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>-1.2409E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2.1585E-2</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>-1.1106E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1.9362999999999998E-2</v>
       </c>
@@ -5231,7 +5231,7 @@
         <v>-1.0659999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1.7412E-2</v>
       </c>
@@ -5341,7 +5341,7 @@
         <v>-1.0090999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1.5740000000000001E-2</v>
       </c>
@@ -5451,7 +5451,7 @@
         <v>-9.4520000000000003E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1.4527E-2</v>
       </c>
@@ -5561,7 +5561,7 @@
         <v>-9.214E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1.379E-2</v>
       </c>
@@ -5671,7 +5671,7 @@
         <v>-9.1629999999999993E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1.2543E-2</v>
       </c>
@@ -5781,7 +5781,7 @@
         <v>-9.1640000000000003E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1.1979999999999999E-2</v>
       </c>
@@ -5891,7 +5891,7 @@
         <v>-9.2560000000000003E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1.141E-2</v>
       </c>
@@ -6001,7 +6001,7 @@
         <v>-9.3310000000000008E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1.0869999999999999E-2</v>
       </c>
@@ -6111,7 +6111,7 @@
         <v>-9.4339999999999997E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1.0403000000000001E-2</v>
       </c>
@@ -6221,7 +6221,7 @@
         <v>-9.6699999999999998E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1.018E-2</v>
       </c>
@@ -6331,7 +6331,7 @@
         <v>-9.9600000000000001E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>9.5879999999999993E-3</v>
       </c>
@@ -6441,7 +6441,7 @@
         <v>-9.9190000000000007E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>9.384E-3</v>
       </c>
@@ -6551,7 +6551,7 @@
         <v>-1.0031999999999999E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>9.025E-3</v>
       </c>
@@ -6661,7 +6661,7 @@
         <v>-9.8969999999999995E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>8.5540000000000008E-3</v>
       </c>
@@ -6771,7 +6771,7 @@
         <v>-9.5949999999999994E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>8.3199999999999993E-3</v>
       </c>
@@ -6881,7 +6881,7 @@
         <v>-9.2449999999999997E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>7.9459999999999999E-3</v>
       </c>
@@ -6991,7 +6991,7 @@
         <v>-8.9110000000000005E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>7.5760000000000003E-3</v>
       </c>
@@ -7101,7 +7101,7 @@
         <v>-8.286E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>7.5640000000000004E-3</v>
       </c>
@@ -7211,7 +7211,7 @@
         <v>-7.8480000000000008E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>7.2570000000000004E-3</v>
       </c>
@@ -7321,7 +7321,7 @@
         <v>-7.273E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>7.1209999999999997E-3</v>
       </c>
@@ -7431,7 +7431,7 @@
         <v>-6.6730000000000001E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7.1009999999999997E-3</v>
       </c>
@@ -7541,7 +7541,7 @@
         <v>-6.0819999999999997E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>6.9690000000000004E-3</v>
       </c>
@@ -7651,7 +7651,7 @@
         <v>-5.555E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>7.1580000000000003E-3</v>
       </c>
@@ -7761,7 +7761,7 @@
         <v>-5.0730000000000003E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>7.0470000000000003E-3</v>
       </c>
@@ -7871,7 +7871,7 @@
         <v>-4.6169999999999996E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>7.2830000000000004E-3</v>
       </c>
@@ -7981,7 +7981,7 @@
         <v>-4.3220000000000003E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>7.0229999999999997E-3</v>
       </c>
@@ -8091,7 +8091,7 @@
         <v>-4.0289999999999996E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>6.6090000000000003E-3</v>
       </c>
@@ -8201,7 +8201,7 @@
         <v>-3.7910000000000001E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>6.4440000000000001E-3</v>
       </c>
@@ -8311,7 +8311,7 @@
         <v>-3.5990000000000002E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>5.9170000000000004E-3</v>
       </c>
@@ -8421,7 +8421,7 @@
         <v>-3.4169999999999999E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1.9090000000000001E-3</v>
       </c>
@@ -8531,7 +8531,7 @@
         <v>-4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1.421E-3</v>
       </c>
@@ -8641,7 +8641,7 @@
         <v>-1.9699999999999999E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1.3699999999999999E-3</v>
       </c>
@@ -8751,7 +8751,7 @@
         <v>6.6000000000000005E-5</v>
       </c>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>9.7599999999999998E-4</v>
       </c>
@@ -8861,7 +8861,7 @@
         <v>3.4499999999999998E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>5.5900000000000004E-4</v>
       </c>
@@ -8971,7 +8971,7 @@
         <v>6.4800000000000003E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>-1.1E-5</v>
       </c>
@@ -9081,7 +9081,7 @@
         <v>1.0020000000000001E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>-5.62E-4</v>
       </c>
@@ -9191,7 +9191,7 @@
         <v>1.3500000000000001E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>-1.3389999999999999E-3</v>
       </c>
@@ -9301,7 +9301,7 @@
         <v>1.5380000000000001E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>-2.0699999999999998E-3</v>
       </c>
@@ -9411,7 +9411,7 @@
         <v>1.722E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>-2.702E-3</v>
       </c>
@@ -9521,7 +9521,7 @@
         <v>1.714E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>-2.8639999999999998E-3</v>
       </c>
@@ -9631,7 +9631,7 @@
         <v>1.7279999999999999E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>-2.9510000000000001E-3</v>
       </c>
@@ -9741,7 +9741,7 @@
         <v>1.5299999999999999E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>-2.8219999999999999E-3</v>
       </c>
@@ -9851,7 +9851,7 @@
         <v>1.3780000000000001E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>-2.7550000000000001E-3</v>
       </c>
@@ -9961,7 +9961,7 @@
         <v>1.0640000000000001E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>-2.5140000000000002E-3</v>
       </c>
@@ -10071,7 +10071,7 @@
         <v>9.3599999999999998E-4</v>
       </c>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>-2.2439999999999999E-3</v>
       </c>
@@ -10181,7 +10181,7 @@
         <v>8.25E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>-2.0070000000000001E-3</v>
       </c>
@@ -10291,7 +10291,7 @@
         <v>6.9899999999999997E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>-1.7780000000000001E-3</v>
       </c>
@@ -10401,7 +10401,7 @@
         <v>6.3199999999999997E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>-1.655E-3</v>
       </c>
@@ -10511,7 +10511,7 @@
         <v>4.6700000000000002E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>-1.6310000000000001E-3</v>
       </c>
@@ -10621,7 +10621,7 @@
         <v>3.2499999999999999E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>-1.5989999999999999E-3</v>
       </c>
@@ -10731,7 +10731,7 @@
         <v>1.93E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>-1.493E-3</v>
       </c>
@@ -10841,7 +10841,7 @@
         <v>6.4999999999999994E-5</v>
       </c>
     </row>
-    <row r="65" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>-1.273E-3</v>
       </c>
@@ -10951,7 +10951,7 @@
         <v>-7.4999999999999993E-5</v>
       </c>
     </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>-1.0189999999999999E-3</v>
       </c>
@@ -11061,7 +11061,7 @@
         <v>-1.5899999999999999E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>-7.1699999999999997E-4</v>
       </c>
@@ -11171,7 +11171,7 @@
         <v>-1.7000000000000001E-4</v>
       </c>
     </row>
-    <row r="68" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>-1.8E-5</v>
       </c>
@@ -11281,7 +11281,7 @@
         <v>-3.1100000000000002E-4</v>
       </c>
     </row>
-    <row r="69" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>3.28E-4</v>
       </c>
@@ -11391,7 +11391,7 @@
         <v>-5.0299999999999997E-4</v>
       </c>
     </row>
-    <row r="70" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>5.8299999999999997E-4</v>
       </c>
@@ -11501,7 +11501,7 @@
         <v>-6.7100000000000005E-4</v>
       </c>
     </row>
-    <row r="71" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>8.4999999999999995E-4</v>
       </c>
@@ -11611,7 +11611,7 @@
         <v>-9.0499999999999999E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1.165E-3</v>
       </c>
@@ -11721,7 +11721,7 @@
         <v>-1.168E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1.469E-3</v>
       </c>
@@ -11831,7 +11831,7 @@
         <v>-1.3760000000000001E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1.9949999999999998E-3</v>
       </c>
@@ -11941,7 +11941,7 @@
         <v>-1.586E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2.3739999999999998E-3</v>
       </c>
@@ -12051,7 +12051,7 @@
         <v>-1.663E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2.3760000000000001E-3</v>
       </c>
@@ -12161,7 +12161,7 @@
         <v>-1.732E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2.4130000000000002E-3</v>
       </c>
@@ -12271,7 +12271,7 @@
         <v>-1.681E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2.166E-3</v>
       </c>
@@ -12381,7 +12381,7 @@
         <v>-1.699E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>1.9530000000000001E-3</v>
       </c>
@@ -12491,7 +12491,7 @@
         <v>-1.627E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>1.7539999999999999E-3</v>
       </c>
@@ -12601,7 +12601,7 @@
         <v>-1.565E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1.653E-3</v>
       </c>
@@ -12711,7 +12711,7 @@
         <v>-1.4779999999999999E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1.4339999999999999E-3</v>
       </c>
@@ -12821,7 +12821,7 @@
         <v>-1.253E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>1.5529999999999999E-3</v>
       </c>
@@ -12931,7 +12931,7 @@
         <v>-1.103E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>1.704E-3</v>
       </c>
@@ -13041,7 +13041,7 @@
         <v>-8.92E-4</v>
       </c>
     </row>
-    <row r="85" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>1.725E-3</v>
       </c>
@@ -13169,9 +13169,9 @@
       <selection activeCell="O106" sqref="O106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0.11464299999999999</v>
       </c>
@@ -13281,7 +13281,7 @@
         <v>-5.0855999999999998E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.11143699999999999</v>
       </c>
@@ -13391,7 +13391,7 @@
         <v>-4.8311E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.10566</v>
       </c>
@@ -13501,7 +13501,7 @@
         <v>-4.7612000000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.103315</v>
       </c>
@@ -13611,7 +13611,7 @@
         <v>-4.4401000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.100078</v>
       </c>
@@ -13721,7 +13721,7 @@
         <v>-4.3917999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9.7517999999999994E-2</v>
       </c>
@@ -13831,7 +13831,7 @@
         <v>-4.0932999999999997E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9.4977000000000006E-2</v>
       </c>
@@ -13941,7 +13941,7 @@
         <v>-3.9729E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9.2086000000000001E-2</v>
       </c>
@@ -14051,7 +14051,7 @@
         <v>-3.8157999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8.8232000000000005E-2</v>
       </c>
@@ -14161,7 +14161,7 @@
         <v>-3.6015999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8.4955000000000003E-2</v>
       </c>
@@ -14271,7 +14271,7 @@
         <v>-3.3876000000000003E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8.2607E-2</v>
       </c>
@@ -14381,7 +14381,7 @@
         <v>-3.2259999999999997E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>7.9913999999999999E-2</v>
       </c>
@@ -14491,7 +14491,7 @@
         <v>-3.0206E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7.8973000000000002E-2</v>
       </c>
@@ -14601,7 +14601,7 @@
         <v>-2.8332E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7.6024999999999995E-2</v>
       </c>
@@ -14711,7 +14711,7 @@
         <v>-2.6426000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7.4902999999999997E-2</v>
       </c>
@@ -14821,7 +14821,7 @@
         <v>-2.4596E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>7.3431999999999997E-2</v>
       </c>
@@ -14931,7 +14931,7 @@
         <v>-2.2771E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>7.2954000000000005E-2</v>
       </c>
@@ -15041,7 +15041,7 @@
         <v>-2.1378000000000001E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>7.2392999999999999E-2</v>
       </c>
@@ -15151,7 +15151,7 @@
         <v>-2.0163E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>7.1642999999999998E-2</v>
       </c>
@@ -15261,7 +15261,7 @@
         <v>-1.9016999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>7.0186999999999999E-2</v>
       </c>
@@ -15371,7 +15371,7 @@
         <v>-1.8008E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6.9302000000000002E-2</v>
       </c>
@@ -15481,7 +15481,7 @@
         <v>-1.7052000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>6.8472000000000005E-2</v>
       </c>
@@ -15591,7 +15591,7 @@
         <v>-1.6406E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6.7325999999999997E-2</v>
       </c>
@@ -15701,7 +15701,7 @@
         <v>-1.5685000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6.6239999999999993E-2</v>
       </c>
@@ -15811,7 +15811,7 @@
         <v>-1.5491E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6.5568000000000001E-2</v>
       </c>
@@ -15921,7 +15921,7 @@
         <v>-1.5266999999999999E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6.4459000000000002E-2</v>
       </c>
@@ -16031,7 +16031,7 @@
         <v>-1.5446E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>6.3698000000000005E-2</v>
       </c>
@@ -16141,7 +16141,7 @@
         <v>-1.5762000000000002E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6.2205000000000003E-2</v>
       </c>
@@ -16251,7 +16251,7 @@
         <v>-1.5906E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6.1772000000000001E-2</v>
       </c>
@@ -16361,7 +16361,7 @@
         <v>-1.6376000000000002E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6.0983000000000002E-2</v>
       </c>
@@ -16471,7 +16471,7 @@
         <v>-1.6698000000000001E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>5.9484000000000002E-2</v>
       </c>
@@ -16581,7 +16581,7 @@
         <v>-1.7065E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>5.885E-2</v>
       </c>
@@ -16691,7 +16691,7 @@
         <v>-1.7538000000000002E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>5.8035000000000003E-2</v>
       </c>
@@ -16801,7 +16801,7 @@
         <v>-1.7956E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>5.6728000000000001E-2</v>
       </c>
@@ -16911,7 +16911,7 @@
         <v>-1.8258E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>5.6006E-2</v>
       </c>
@@ -17021,7 +17021,7 @@
         <v>-1.8557000000000001E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>5.4544000000000002E-2</v>
       </c>
@@ -17131,7 +17131,7 @@
         <v>-1.8412999999999999E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>5.3428000000000003E-2</v>
       </c>
@@ -17241,7 +17241,7 @@
         <v>-1.8096000000000001E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>5.2255000000000003E-2</v>
       </c>
@@ -17351,7 +17351,7 @@
         <v>-1.7731E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>5.1347999999999998E-2</v>
       </c>
@@ -17461,7 +17461,7 @@
         <v>-1.7405E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>5.0941E-2</v>
       </c>
@@ -17571,7 +17571,7 @@
         <v>-1.6965000000000001E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>5.0456000000000001E-2</v>
       </c>
@@ -17681,7 +17681,7 @@
         <v>-1.6688000000000001E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>4.9521000000000003E-2</v>
       </c>
@@ -17791,7 +17791,7 @@
         <v>-1.6479000000000001E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>5.2349E-2</v>
       </c>
@@ -17901,7 +17901,7 @@
         <v>-1.9583E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>5.2712000000000002E-2</v>
       </c>
@@ -18011,7 +18011,7 @@
         <v>-1.9982E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>5.2965999999999999E-2</v>
       </c>
@@ -18121,7 +18121,7 @@
         <v>-2.0264000000000001E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>5.373E-2</v>
       </c>
@@ -18231,7 +18231,7 @@
         <v>-2.0386000000000001E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>5.4421999999999998E-2</v>
       </c>
@@ -18341,7 +18341,7 @@
         <v>-2.0745E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>5.5028000000000001E-2</v>
       </c>
@@ -18451,7 +18451,7 @@
         <v>-2.0560999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>5.5216000000000001E-2</v>
       </c>
@@ -18561,7 +18561,7 @@
         <v>-2.0379999999999999E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>5.5146000000000001E-2</v>
       </c>
@@ -18671,7 +18671,7 @@
         <v>-1.9935000000000001E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>5.4336000000000002E-2</v>
       </c>
@@ -18781,7 +18781,7 @@
         <v>-1.9289000000000001E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>5.3359999999999998E-2</v>
       </c>
@@ -18891,7 +18891,7 @@
         <v>-1.8554999999999999E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>5.2211E-2</v>
       </c>
@@ -19001,7 +19001,7 @@
         <v>-1.8151E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>5.0758999999999999E-2</v>
       </c>
@@ -19111,7 +19111,7 @@
         <v>-1.7795999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>4.9699E-2</v>
       </c>
@@ -19221,7 +19221,7 @@
         <v>-1.7281000000000001E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>4.9028000000000002E-2</v>
       </c>
@@ -19331,7 +19331,7 @@
         <v>-1.6966999999999999E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>4.8057000000000002E-2</v>
       </c>
@@ -19441,7 +19441,7 @@
         <v>-1.6674999999999999E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>4.7393999999999999E-2</v>
       </c>
@@ -19551,7 +19551,7 @@
         <v>-1.6372000000000001E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>4.6948999999999998E-2</v>
       </c>
@@ -19661,7 +19661,7 @@
         <v>-1.6211E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>4.6358000000000003E-2</v>
       </c>
@@ -19771,7 +19771,7 @@
         <v>-1.5982E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>4.6005999999999998E-2</v>
       </c>
@@ -19881,7 +19881,7 @@
         <v>-1.5730999999999998E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>4.5657000000000003E-2</v>
       </c>
@@ -19991,7 +19991,7 @@
         <v>-1.5650000000000001E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>4.4887999999999997E-2</v>
       </c>
@@ -20101,7 +20101,7 @@
         <v>-1.5442000000000001E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>4.4344000000000001E-2</v>
       </c>
@@ -20211,7 +20211,7 @@
         <v>-1.5474999999999999E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>4.3698000000000001E-2</v>
       </c>
@@ -20321,7 +20321,7 @@
         <v>-1.5446E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>4.2992000000000002E-2</v>
       </c>
@@ -20431,7 +20431,7 @@
         <v>-1.5382E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>4.2221000000000002E-2</v>
       </c>
@@ -20541,7 +20541,7 @@
         <v>-1.5272000000000001E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>4.2258999999999998E-2</v>
       </c>
@@ -20651,7 +20651,7 @@
         <v>-1.5022000000000001E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>4.1813000000000003E-2</v>
       </c>
@@ -20761,7 +20761,7 @@
         <v>-1.4598E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>4.1190999999999998E-2</v>
       </c>
@@ -20871,7 +20871,7 @@
         <v>-1.439E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>4.1315999999999999E-2</v>
       </c>
@@ -20981,7 +20981,7 @@
         <v>-1.4239E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>4.0593999999999998E-2</v>
       </c>
@@ -21091,7 +21091,7 @@
         <v>-1.4161E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>4.0902000000000001E-2</v>
       </c>
@@ -21201,7 +21201,7 @@
         <v>-1.4272999999999999E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>4.0507000000000001E-2</v>
       </c>
@@ -21311,7 +21311,7 @@
         <v>-1.4279999999999999E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>4.1043999999999997E-2</v>
       </c>
@@ -21421,7 +21421,7 @@
         <v>-1.4352999999999999E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>4.0555000000000001E-2</v>
       </c>
@@ -21531,7 +21531,7 @@
         <v>-1.4429000000000001E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>4.1255E-2</v>
       </c>
@@ -21641,7 +21641,7 @@
         <v>-1.4637000000000001E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>4.0912999999999998E-2</v>
       </c>
@@ -21751,7 +21751,7 @@
         <v>-1.4713E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>4.1392999999999999E-2</v>
       </c>
@@ -21861,7 +21861,7 @@
         <v>-1.5044E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>4.0951000000000001E-2</v>
       </c>
@@ -21971,7 +21971,7 @@
         <v>-1.5200999999999999E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>4.0934999999999999E-2</v>
       </c>
@@ -22081,7 +22081,7 @@
         <v>-1.54E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>4.0092999999999997E-2</v>
       </c>
@@ -22191,7 +22191,7 @@
         <v>-1.5492000000000001E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>3.9625E-2</v>
       </c>
@@ -22301,7 +22301,7 @@
         <v>-1.5389E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>3.8066000000000003E-2</v>
       </c>
@@ -22411,7 +22411,7 @@
         <v>-1.4987E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>3.8646E-2</v>
       </c>

</xml_diff>